<commit_message>
bug in format_excel_header intriduced
</commit_message>
<xml_diff>
--- a/data/output/processed_loan_data.xlsx
+++ b/data/output/processed_loan_data.xlsx
@@ -29,12 +29,18 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -55,11 +61,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -481,35 +488,35 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="2" t="n">
         <v>101</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>Alice</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" s="2" t="n">
         <v>50000</v>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
         <is>
           <t>Personal</t>
         </is>
       </c>
-      <c r="E2" t="n">
+      <c r="E2" s="2" t="n">
         <v>0.05</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="G2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
+      <c r="G2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2" t="n">
         <v>62500</v>
       </c>
-      <c r="I2" t="b">
+      <c r="I2" s="2" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>